<commit_message>
Serialization for 'Problem' and 'Solution' in Modules FAQ
</commit_message>
<xml_diff>
--- a/Assets/SMILocalization.xlsx
+++ b/Assets/SMILocalization.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>key</t>
   </si>
@@ -235,6 +235,21 @@
   </si>
   <si>
     <t>Try a bit harder next time</t>
+  </si>
+  <si>
+    <t>PROBLEM</t>
+  </si>
+  <si>
+    <t>SOLUTION</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>PROBLEEM</t>
+  </si>
+  <si>
+    <t>Oplossing</t>
   </si>
 </sst>
 </file>
@@ -560,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,7 +586,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,6 +890,28 @@
         <v>44</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="42" ht="13.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="48" ht="13.4" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>